<commit_message>
Refactored schematic for I2C IO expander and ADCs.
This commit in anticipation of offboard current monitoring through motor drivers and current sense board.
</commit_message>
<xml_diff>
--- a/Design/i2c_addresses.xlsx
+++ b/Design/i2c_addresses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\rackstation\media\documents\Inventor\AutoBuoy\design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\CreekFleet_AutoBuoy\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB123CE-D8B0-414A-8AAF-7F71A34FC915}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19410E6-29B0-4528-9756-2F06270C69A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{18B35A54-1527-46B2-B18B-0B33FD9D2257}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18B35A54-1527-46B2-B18B-0B33FD9D2257}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>A1</t>
   </si>
@@ -45,27 +45,6 @@
     <t>Hex</t>
   </si>
   <si>
-    <t>1000001</t>
-  </si>
-  <si>
-    <t>1000010</t>
-  </si>
-  <si>
-    <t>1000011</t>
-  </si>
-  <si>
-    <t>1000100</t>
-  </si>
-  <si>
-    <t>1000101</t>
-  </si>
-  <si>
-    <t>1000110</t>
-  </si>
-  <si>
-    <t>1000111</t>
-  </si>
-  <si>
     <t>1001000</t>
   </si>
   <si>
@@ -78,18 +57,6 @@
     <t>1001011</t>
   </si>
   <si>
-    <t>1001100</t>
-  </si>
-  <si>
-    <t>1001101</t>
-  </si>
-  <si>
-    <t>1001110</t>
-  </si>
-  <si>
-    <t>1001111</t>
-  </si>
-  <si>
     <t>GND</t>
   </si>
   <si>
@@ -108,29 +75,47 @@
     <t>Function</t>
   </si>
   <si>
-    <t>INA219</t>
-  </si>
-  <si>
-    <t>VBATT</t>
-  </si>
-  <si>
-    <t>Left Motor</t>
-  </si>
-  <si>
-    <t>Right Motor</t>
-  </si>
-  <si>
-    <t>Winch Motor</t>
+    <t>ADS1015</t>
+  </si>
+  <si>
+    <t>currents</t>
+  </si>
+  <si>
+    <t>1111000</t>
+  </si>
+  <si>
+    <t>OLED</t>
+  </si>
+  <si>
+    <t>display</t>
+  </si>
+  <si>
+    <t>voltages</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>MCP23017</t>
+  </si>
+  <si>
+    <t>GPIO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,9 +141,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,14 +170,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A049DA6-5770-4993-8F8F-7FE2393B61D6}" name="Table1" displayName="Table1" ref="A1:F17" totalsRowShown="0">
-  <autoFilter ref="A1:F17" xr:uid="{E1326F2E-1307-4A1A-849A-F068C455CAB9}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C68A0BEE-674A-4355-AB52-4CC0AE47C1EB}" name="A1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A049DA6-5770-4993-8F8F-7FE2393B61D6}" name="Table1" displayName="Table1" ref="A1:G7" totalsRowShown="0">
+  <autoFilter ref="A1:G7" xr:uid="{E1326F2E-1307-4A1A-849A-F068C455CAB9}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{AC739AC0-EC59-466B-B2B3-979117A98D25}" name="A2"/>
+    <tableColumn id="7" xr3:uid="{F3B2DF9A-E735-495A-8625-0560F8697187}" name="A1"/>
     <tableColumn id="2" xr3:uid="{A3541604-30E2-48E3-8C90-D76498185AD4}" name="A0"/>
     <tableColumn id="3" xr3:uid="{6777B4A7-BD80-4B59-A940-BD9A6CBBF087}" name="Address" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{06A3B895-0CF4-4F55-9C0C-5D9834ECBC78}" name="Hex" dataDxfId="0">
-      <calculatedColumnFormula>_xlfn.CONCAT("0x",BIN2HEX(C2,2))</calculatedColumnFormula>
+      <calculatedColumnFormula>_xlfn.CONCAT("0x",BIN2HEX(D2,2))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{14D089C4-ECC1-40AB-9C14-2526AC2F45E4}" name="Device"/>
     <tableColumn id="6" xr3:uid="{99889B9B-6E58-491E-8224-EA71C721F873}" name="Function"/>
@@ -497,309 +484,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9064D9C-9EED-43D1-8F62-0FAD39ACE94C}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="D2" t="str">
-        <f t="shared" ref="D2:D17" si="0">_xlfn.CONCAT("0x",BIN2HEX(C2,2))</f>
-        <v>0x40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2"/>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E5" si="0">_xlfn.CONCAT("0x",BIN2HEX(D2,2))</f>
+        <v>0x48</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" si="0"/>
-        <v>0x41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3"/>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v>0x42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>0x43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>0x44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>0x45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>0x46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>0x47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>0x48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="str">
+      <c r="E3" t="str">
         <f t="shared" si="0"/>
         <v>0x49</v>
       </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="str">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4"/>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="str">
         <f t="shared" si="0"/>
         <v>0x4A</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="str">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5"/>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="str">
         <f t="shared" si="0"/>
         <v>0x4B</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6"/>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f>_xlfn.CONCAT("0x",BIN2HEX(D6,2))</f>
+        <v>0x78</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f>_xlfn.CONCAT("0100",IF(Table1[[#This Row],[A2]]="VCC",1,0),IF(Table1[[#This Row],[A1]]="VCC",1,0),IF(Table1[[#This Row],[A0]]="VCC",1,0))</f>
+        <v>0100000</v>
+      </c>
+      <c r="E7" s="2" t="str">
+        <f>_xlfn.CONCAT("0x",BIN2HEX(D7,2))</f>
+        <v>0x20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
         <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v>0x4C</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v>0x4D</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>0x4E</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v>0x4F</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed board art. Pending external review.
</commit_message>
<xml_diff>
--- a/Design/i2c_addresses.xlsx
+++ b/Design/i2c_addresses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\CreekFleet_AutoBuoy\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19410E6-29B0-4528-9756-2F06270C69A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72443CAF-DC33-4247-A291-76B0E3F63A55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18B35A54-1527-46B2-B18B-0B33FD9D2257}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18B35A54-1527-46B2-B18B-0B33FD9D2257}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>A1</t>
   </si>
@@ -51,24 +51,12 @@
     <t>1001001</t>
   </si>
   <si>
-    <t>1001010</t>
-  </si>
-  <si>
-    <t>1001011</t>
-  </si>
-  <si>
     <t>GND</t>
   </si>
   <si>
     <t>VCC</t>
   </si>
   <si>
-    <t>SDA</t>
-  </si>
-  <si>
-    <t>SCL</t>
-  </si>
-  <si>
     <t>Device</t>
   </si>
   <si>
@@ -100,6 +88,15 @@
   </si>
   <si>
     <t>GPIO</t>
+  </si>
+  <si>
+    <t>DS3231</t>
+  </si>
+  <si>
+    <t>RTC</t>
+  </si>
+  <si>
+    <t>1101000</t>
   </si>
 </sst>
 </file>
@@ -170,8 +167,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A049DA6-5770-4993-8F8F-7FE2393B61D6}" name="Table1" displayName="Table1" ref="A1:G7" totalsRowShown="0">
-  <autoFilter ref="A1:G7" xr:uid="{E1326F2E-1307-4A1A-849A-F068C455CAB9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A049DA6-5770-4993-8F8F-7FE2393B61D6}" name="Table1" displayName="Table1" ref="A1:G6" totalsRowShown="0">
+  <autoFilter ref="A1:G6" xr:uid="{E1326F2E-1307-4A1A-849A-F068C455CAB9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G6">
+    <sortCondition ref="E1:E6"/>
+  </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{AC739AC0-EC59-466B-B2B3-979117A98D25}" name="A2"/>
     <tableColumn id="7" xr3:uid="{F3B2DF9A-E735-495A-8625-0560F8697187}" name="A1"/>
@@ -484,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9064D9C-9EED-43D1-8F62-0FAD39ACE94C}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +503,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -518,115 +518,104 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2"/>
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="str">
-        <f t="shared" ref="E2:E5" si="0">_xlfn.CONCAT("0x",BIN2HEX(D2,2))</f>
-        <v>0x48</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f>_xlfn.CONCAT("0100",IF(Table1[[#This Row],[A2]]="VCC",1,0),IF(Table1[[#This Row],[A1]]="VCC",1,0),IF(Table1[[#This Row],[A0]]="VCC",1,0))</f>
+        <v>0100000</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f>_xlfn.CONCAT("0x",BIN2HEX(D2,2))</f>
+        <v>0x20</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3"/>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" si="0"/>
-        <v>0x49</v>
+        <f>_xlfn.CONCAT("0x",BIN2HEX(D3,2))</f>
+        <v>0x48</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4"/>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="str">
+        <f>_xlfn.CONCAT("0x",BIN2HEX(D4,2))</f>
+        <v>0x49</v>
+      </c>
+      <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" si="0"/>
-        <v>0x4A</v>
+      <c r="G4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5"/>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" si="0"/>
-        <v>0x4B</v>
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f>_xlfn.CONCAT("0x",BIN2HEX(D5,2))</f>
+        <v>0x68</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6"/>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E6" s="2" t="str">
         <f>_xlfn.CONCAT("0x",BIN2HEX(D6,2))</f>
         <v>0x78</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2" t="str">
-        <f>_xlfn.CONCAT("0100",IF(Table1[[#This Row],[A2]]="VCC",1,0),IF(Table1[[#This Row],[A1]]="VCC",1,0),IF(Table1[[#This Row],[A0]]="VCC",1,0))</f>
-        <v>0100000</v>
-      </c>
-      <c r="E7" s="2" t="str">
-        <f>_xlfn.CONCAT("0x",BIN2HEX(D7,2))</f>
-        <v>0x20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>